<commit_message>
working touchgfx with board
</commit_message>
<xml_diff>
--- a/Dashboard_Modules/TouchGFX/assets/texts/texts.xlsx
+++ b/Dashboard_Modules/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2520" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2640" uniqueCount="92">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -288,6 +288,9 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId18</t>
   </si>
 </sst>
 </file>
@@ -1964,6 +1967,23 @@
         <v>67</v>
       </c>
     </row>
+    <row r="18">
+      <c r="B18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>